<commit_message>
adding phase lock settings
</commit_message>
<xml_diff>
--- a/config/acquisitionConfig/roi.csv.xlsx
+++ b/config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="513">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1507,6 +1507,78 @@
   </si>
   <si>
     <t>[800 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BecCameraSBB</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
   </si>
 </sst>
 </file>
@@ -1993,19 +2065,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>369</v>
+        <v>489</v>
       </c>
       <c r="B5" s="0">
-        <v>911</v>
+        <v>896</v>
       </c>
       <c r="C5" s="0">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D5" s="0">
-        <v>1235</v>
+        <v>1161</v>
       </c>
       <c r="E5" s="0">
-        <v>1511</v>
+        <v>1453</v>
       </c>
       <c r="F5" s="0">
         <v>2160</v>
@@ -2017,62 +2089,65 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>370</v>
+        <v>490</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>371</v>
+        <v>491</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>372</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>301</v>
-      </c>
-      <c r="C6">
-        <v>645</v>
-      </c>
-      <c r="D6">
-        <v>654</v>
-      </c>
-      <c r="E6">
-        <v>1018</v>
-      </c>
-      <c r="F6">
+      <c r="A6" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B6" s="0">
+        <v>436</v>
+      </c>
+      <c r="C6" s="0">
+        <v>562</v>
+      </c>
+      <c r="D6" s="0">
+        <v>825</v>
+      </c>
+      <c r="E6" s="0">
+        <v>963</v>
+      </c>
+      <c r="F6" s="0">
         <v>1080</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>1920</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
+      <c r="I6" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>365</v>
+        <v>509</v>
       </c>
       <c r="B7" s="0">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="C7" s="0">
-        <v>1372</v>
+        <v>1393</v>
       </c>
       <c r="D7" s="0">
-        <v>1286</v>
+        <v>1233</v>
       </c>
       <c r="E7" s="0">
-        <v>1442</v>
+        <v>1369</v>
       </c>
       <c r="F7" s="0">
         <v>2160</v>
@@ -2084,13 +2159,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>366</v>
+        <v>510</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>367</v>
+        <v>511</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>368</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8">
@@ -2515,19 +2590,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>89</v>
+        <v>497</v>
       </c>
       <c r="B20" s="0">
-        <v>243</v>
+        <v>447</v>
       </c>
       <c r="C20" s="0">
-        <v>583</v>
+        <v>735</v>
       </c>
       <c r="D20" s="0">
-        <v>678</v>
+        <v>921</v>
       </c>
       <c r="E20" s="0">
-        <v>988</v>
+        <v>1203</v>
       </c>
       <c r="F20" s="0">
         <v>1080</v>
@@ -2539,13 +2614,13 @@
         <v>0</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>90</v>
+        <v>498</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>91</v>
+        <v>499</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>92</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21">

</xml_diff>